<commit_message>
Add model assets for all models, Add model metrics for Type 2 and 7
</commit_message>
<xml_diff>
--- a/models/types1-24/AllModels.xlsx
+++ b/models/types1-24/AllModels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/colbyford/Documents/pfHRP_MLModel/models/types1-24/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Colby\Documents\GitHub\pfHRP_MLModel\models\types1-24\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0C60682D-BCAF-3F4F-870A-5B2FE7B5DD92}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02C52712-738B-4FD5-A8C6-6CE402338AE6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="15840" xr2:uid="{56B93907-60D1-8B42-B22A-F58A3AADB790}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{56B93907-60D1-8B42-B22A-F58A3AADB790}"/>
   </bookViews>
   <sheets>
     <sheet name="pfHRP2_Types1-24" sheetId="2" r:id="rId1"/>
@@ -99,25 +99,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF373737"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -140,10 +128,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -461,16 +447,16 @@
   <dimension ref="A1:C65"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B60" sqref="B60"/>
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="40.6640625" customWidth="1"/>
-    <col min="2" max="2" width="40.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="18.875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -481,701 +467,701 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1">
+      <c r="C2">
         <v>0.81845000000000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>6</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3">
         <v>0.81201999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
       <c r="B4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4">
         <v>0.80654999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>6</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5">
         <v>0.80654999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>6</v>
       </c>
       <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6">
         <v>0.80274000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C7">
         <v>0.80274000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="1">
+      <c r="C8">
         <v>0.77988000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>6</v>
       </c>
       <c r="B9" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1">
+      <c r="C9">
         <v>0.77876999999999996</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>11</v>
       </c>
       <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C10">
         <v>0.77566999999999997</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>11</v>
       </c>
       <c r="B11" t="s">
         <v>5</v>
       </c>
-      <c r="C11" s="1">
+      <c r="C11">
         <v>0.77566999999999997</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>11</v>
       </c>
       <c r="B12" t="s">
         <v>5</v>
       </c>
-      <c r="C12" s="1">
+      <c r="C12">
         <v>0.77566999999999997</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>6</v>
       </c>
       <c r="B13" t="s">
         <v>12</v>
       </c>
-      <c r="C13" s="1">
+      <c r="C13">
         <v>0.77137999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>11</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
       </c>
-      <c r="C14" s="1">
+      <c r="C14">
         <v>0.77059999999999995</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>9</v>
       </c>
-      <c r="C15" s="1">
+      <c r="C15">
         <v>0.76951999999999998</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
       <c r="B16" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="1">
+      <c r="C16">
         <v>0.76951999999999998</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>14</v>
       </c>
       <c r="B17" t="s">
         <v>8</v>
       </c>
-      <c r="C17" s="1">
+      <c r="C17">
         <v>0.76495999999999997</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
         <v>9</v>
       </c>
-      <c r="C18" s="1">
+      <c r="C18">
         <v>0.76114999999999999</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
       <c r="B19" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="1">
+      <c r="C19">
         <v>0.76027</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>14</v>
       </c>
       <c r="B20" t="s">
         <v>5</v>
       </c>
-      <c r="C20" s="1">
+      <c r="C20">
         <v>0.75756999999999997</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
         <v>8</v>
       </c>
-      <c r="C21" s="1">
+      <c r="C21">
         <v>0.75566</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>15</v>
       </c>
-      <c r="C22" s="1">
+      <c r="C22">
         <v>0.75226000000000004</v>
       </c>
     </row>
-    <row r="23" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
       <c r="B23" t="s">
         <v>5</v>
       </c>
-      <c r="C23" s="1">
+      <c r="C23">
         <v>0.75197000000000003</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>13</v>
       </c>
       <c r="B24" t="s">
         <v>5</v>
       </c>
-      <c r="C24" s="1">
+      <c r="C24">
         <v>0.75197000000000003</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
       <c r="B25" t="s">
         <v>5</v>
       </c>
-      <c r="C25" s="1">
+      <c r="C25">
         <v>0.75197000000000003</v>
       </c>
     </row>
-    <row r="26" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>13</v>
       </c>
       <c r="B26" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="1">
+      <c r="C26">
         <v>0.75197000000000003</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
       <c r="B27" t="s">
         <v>5</v>
       </c>
-      <c r="C27" s="1">
+      <c r="C27">
         <v>0.75197000000000003</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>13</v>
       </c>
       <c r="B28" t="s">
         <v>5</v>
       </c>
-      <c r="C28" s="1">
+      <c r="C28">
         <v>0.75197000000000003</v>
       </c>
     </row>
-    <row r="29" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>6</v>
       </c>
       <c r="B29" t="s">
         <v>15</v>
       </c>
-      <c r="C29" s="1">
+      <c r="C29">
         <v>0.74836000000000003</v>
       </c>
     </row>
-    <row r="30" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>6</v>
       </c>
       <c r="B30" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="1">
+      <c r="C30">
         <v>0.74816000000000005</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>6</v>
       </c>
       <c r="B31" t="s">
         <v>9</v>
       </c>
-      <c r="C31" s="1">
+      <c r="C31">
         <v>0.74614000000000003</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>14</v>
       </c>
       <c r="B32" t="s">
         <v>5</v>
       </c>
-      <c r="C32" s="1">
+      <c r="C32">
         <v>0.74455000000000005</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>16</v>
       </c>
       <c r="B33" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="1">
+      <c r="C33">
         <v>0.74056</v>
       </c>
     </row>
-    <row r="34" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>11</v>
       </c>
       <c r="B34" t="s">
         <v>10</v>
       </c>
-      <c r="C34" s="1">
+      <c r="C34">
         <v>0.73860000000000003</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>6</v>
       </c>
       <c r="B35" t="s">
         <v>10</v>
       </c>
-      <c r="C35" s="1">
+      <c r="C35">
         <v>0.73860000000000003</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>14</v>
       </c>
       <c r="B36" t="s">
         <v>5</v>
       </c>
-      <c r="C36" s="1">
+      <c r="C36">
         <v>0.73704999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>6</v>
       </c>
       <c r="B37" t="s">
         <v>5</v>
       </c>
-      <c r="C37" s="1">
+      <c r="C37">
         <v>0.73638999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>14</v>
       </c>
       <c r="B38" t="s">
         <v>8</v>
       </c>
-      <c r="C38" s="1">
+      <c r="C38">
         <v>0.73265000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
       <c r="B39" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="1">
+      <c r="C39">
         <v>0.73245000000000005</v>
       </c>
     </row>
-    <row r="40" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>6</v>
       </c>
       <c r="B40" t="s">
         <v>5</v>
       </c>
-      <c r="C40" s="1">
+      <c r="C40">
         <v>0.73109999999999997</v>
       </c>
     </row>
-    <row r="41" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>14</v>
       </c>
       <c r="B41" t="s">
         <v>15</v>
       </c>
-      <c r="C41" s="1">
+      <c r="C41">
         <v>0.73019999999999996</v>
       </c>
     </row>
-    <row r="42" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>6</v>
       </c>
       <c r="B42" t="s">
         <v>5</v>
       </c>
-      <c r="C42" s="2">
+      <c r="C42">
         <v>0.72789000000000004</v>
       </c>
     </row>
-    <row r="43" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>14</v>
       </c>
       <c r="B43" t="s">
         <v>8</v>
       </c>
-      <c r="C43" s="1">
+      <c r="C43">
         <v>0.72463999999999995</v>
       </c>
     </row>
-    <row r="44" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>14</v>
       </c>
       <c r="B44" t="s">
         <v>15</v>
       </c>
-      <c r="C44" s="1">
+      <c r="C44">
         <v>0.72074000000000005</v>
       </c>
     </row>
-    <row r="45" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>17</v>
       </c>
       <c r="B45" t="s">
         <v>8</v>
       </c>
-      <c r="C45" s="1">
+      <c r="C45">
         <v>0.71638999999999997</v>
       </c>
     </row>
-    <row r="46" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>18</v>
       </c>
       <c r="B46" t="s">
         <v>8</v>
       </c>
-      <c r="C46" s="1">
+      <c r="C46">
         <v>0.71035999999999999</v>
       </c>
     </row>
-    <row r="47" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>14</v>
       </c>
       <c r="B47" t="s">
         <v>8</v>
       </c>
-      <c r="C47" s="1">
+      <c r="C47">
         <v>0.70884000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>14</v>
       </c>
       <c r="B48" t="s">
         <v>5</v>
       </c>
-      <c r="C48" s="1">
+      <c r="C48">
         <v>0.70877000000000001</v>
       </c>
     </row>
-    <row r="49" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>11</v>
       </c>
       <c r="B49" t="s">
         <v>15</v>
       </c>
-      <c r="C49" s="1">
+      <c r="C49">
         <v>0.70769000000000004</v>
       </c>
     </row>
-    <row r="50" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>11</v>
       </c>
       <c r="B50" t="s">
         <v>15</v>
       </c>
-      <c r="C50" s="1">
+      <c r="C50">
         <v>0.70530999999999999</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>13</v>
       </c>
       <c r="B51" t="s">
         <v>5</v>
       </c>
-      <c r="C51" s="1">
+      <c r="C51">
         <v>0.70328000000000002</v>
       </c>
     </row>
-    <row r="52" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>11</v>
       </c>
       <c r="B52" t="s">
         <v>15</v>
       </c>
-      <c r="C52" s="1">
+      <c r="C52">
         <v>0.69594999999999996</v>
       </c>
     </row>
-    <row r="53" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>19</v>
       </c>
       <c r="B53" t="s">
         <v>8</v>
       </c>
-      <c r="C53" s="1">
+      <c r="C53">
         <v>0.69220999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>6</v>
       </c>
       <c r="B54" t="s">
         <v>5</v>
       </c>
-      <c r="C54" s="1">
+      <c r="C54">
         <v>0.68722000000000005</v>
       </c>
     </row>
-    <row r="55" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>14</v>
       </c>
       <c r="B55" t="s">
         <v>9</v>
       </c>
-      <c r="C55" s="1">
+      <c r="C55">
         <v>0.67091000000000001</v>
       </c>
     </row>
-    <row r="56" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>11</v>
       </c>
       <c r="B56" t="s">
         <v>5</v>
       </c>
-      <c r="C56" s="1">
+      <c r="C56">
         <v>0.64705000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>14</v>
       </c>
       <c r="B57" t="s">
         <v>5</v>
       </c>
-      <c r="C57" s="1">
+      <c r="C57">
         <v>0.62673000000000001</v>
       </c>
     </row>
-    <row r="58" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>11</v>
       </c>
       <c r="B58" t="s">
         <v>15</v>
       </c>
-      <c r="C58" s="1">
+      <c r="C58">
         <v>0.61468999999999996</v>
       </c>
     </row>
-    <row r="59" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>11</v>
       </c>
       <c r="B59" t="s">
         <v>5</v>
       </c>
-      <c r="C59" s="1">
+      <c r="C59">
         <v>0.61160000000000003</v>
       </c>
     </row>
-    <row r="60" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>11</v>
       </c>
       <c r="B60" t="s">
         <v>15</v>
       </c>
-      <c r="C60" s="1">
+      <c r="C60">
         <v>0.59880999999999995</v>
       </c>
     </row>
-    <row r="61" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>6</v>
       </c>
       <c r="B61" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="1">
+      <c r="C61">
         <v>0.59404999999999997</v>
       </c>
     </row>
-    <row r="62" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>1</v>
       </c>
-      <c r="C62" s="1">
+      <c r="C62">
         <v>0.59370999999999996</v>
       </c>
     </row>
-    <row r="63" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>11</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
       </c>
-      <c r="C63" s="1">
+      <c r="C63">
         <v>0.37714999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>19</v>
       </c>
       <c r="B64" t="s">
         <v>7</v>
       </c>
-      <c r="C64" s="1">
+      <c r="C64">
         <v>0.37714999999999999</v>
       </c>
     </row>
-    <row r="65" spans="1:3" ht="21" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>19</v>
       </c>
       <c r="B65" t="s">
         <v>8</v>
       </c>
-      <c r="C65" s="1">
+      <c r="C65">
         <v>0.37714999999999999</v>
       </c>
     </row>

</xml_diff>